<commit_message>
Cooked meals and ingredients XLSX done
</commit_message>
<xml_diff>
--- a/db/helper/xlsx/cooked_meals.xlsx
+++ b/db/helper/xlsx/cooked_meals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="cooked_meals" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -50,21 +50,6 @@
     <t>FILE:cooked_meals_ingredients.csv</t>
   </si>
   <si>
-    <t>Bro</t>
-  </si>
-  <si>
-    <t>Desc</t>
-  </si>
-  <si>
-    <t>Dir</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Thumb</t>
-  </si>
-  <si>
     <t>cooked_meal</t>
   </si>
   <si>
@@ -92,10 +77,205 @@
     <t>Tomato</t>
   </si>
   <si>
-    <t>Stuff</t>
-  </si>
-  <si>
-    <t>Things</t>
+    <t>Vietnamese Sandwiches</t>
+  </si>
+  <si>
+    <t>This part should be done the night before! Thaw the pork shoulder. To quicken the process, leave pork shoulder still in the package with lukewarm water. Wash the pork and pat dry with a paper towel. When done, place pork in a container and cover with the Char Siu sauce and mix. Let it sit over night. The longer it sits, the better the taste. On the next day, preheat oven to 375. Lay pork in aluminum trays and set in oven for 25 to 30 minutes and flip over the pork. Let it bake for another 15-20 minutes. Make sure to check that the inside is cooked. Cut the pork into slices. You can grill the buns if you want to for crispness. During the baking time, wash and cut the cucumbers into half-circles, wash and pull apart the cilantro. Put into sandwiches when ready!</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7111/8160415698_1bb88ae465.jpg</t>
+  </si>
+  <si>
+    <t>Hoagie Rolls</t>
+  </si>
+  <si>
+    <t>Char Siu Sauce</t>
+  </si>
+  <si>
+    <t>Pork Shoulder</t>
+  </si>
+  <si>
+    <t>Shredded Carrots</t>
+  </si>
+  <si>
+    <t>Cilantro</t>
+  </si>
+  <si>
+    <t>Grilled Hotdogs</t>
+  </si>
+  <si>
+    <t>An All-American grilling classic</t>
+  </si>
+  <si>
+    <t>BBQ Pork Vietnamese sandwiches great for lunch</t>
+  </si>
+  <si>
+    <t>Place on grill. Make sure the hot dogs are cooked thoroughly.</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7110/8160415758_6f1c3a38bc.jpg</t>
+  </si>
+  <si>
+    <t>Hot Dog</t>
+  </si>
+  <si>
+    <t>Hot Dog Buns</t>
+  </si>
+  <si>
+    <t>Salmon Bibimbap</t>
+  </si>
+  <si>
+    <t>A Simple Korean meal</t>
+  </si>
+  <si>
+    <t>Oven to 400 degrees. Wash and Cook Rice. Prepare Salmon with light touch of salt &amp; pepper. Cut tofu into 1/2 inch cubes. Wash and cut vegetables. Organize into bowls and you're done!</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8206/8245871658_2e495bef7f_h.jpg</t>
+  </si>
+  <si>
+    <t>Red-Leaf Lettuce</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Green Onions</t>
+  </si>
+  <si>
+    <t>Daikon Sprouts</t>
+  </si>
+  <si>
+    <t>Roasted Seaweed</t>
+  </si>
+  <si>
+    <t>Gochujang (Red Bean Paste)</t>
+  </si>
+  <si>
+    <t>Tofu</t>
+  </si>
+  <si>
+    <t>Miso Paste</t>
+  </si>
+  <si>
+    <t>Sushi Bake</t>
+  </si>
+  <si>
+    <t>A Japanese fusion meal</t>
+  </si>
+  <si>
+    <t>Wash and cook rice. Wash shitake mushrooms until soft and thaw shrimp and imitation crab (if necessary). Wash and chop vegetables and imitation crab. Cook shitake mushrooms with soy sauce and sugar. Mix all vegetables and imitation crab with mayo, sour cream, furikake. In aluminum tray, put a layer of rice with a cover of your mixture (Ratio of 1.5:1, rice:mixture). Sprinkle masago and green onion (optional). Cut seaweed into 4's, chop romaine lettuce into 1-inch pieces and cucumbers into half-circles. Make Salad Dressing with balsamic vinegar, olive oil, soy sauce and sugar</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8068/8244890595_44423ca495.jpg</t>
+  </si>
+  <si>
+    <t>Mayonnaise</t>
+  </si>
+  <si>
+    <t>Sour Cream</t>
+  </si>
+  <si>
+    <t>Shiitake Mushrooms</t>
+  </si>
+  <si>
+    <t>Imitation Crab</t>
+  </si>
+  <si>
+    <t>Shrimp</t>
+  </si>
+  <si>
+    <t>Masago</t>
+  </si>
+  <si>
+    <t>Furikake</t>
+  </si>
+  <si>
+    <t>Romaine Lettuce</t>
+  </si>
+  <si>
+    <t>Balsamic Vinegar</t>
+  </si>
+  <si>
+    <t>Olive Oil</t>
+  </si>
+  <si>
+    <t>Soy Sauce</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>California Roll</t>
+  </si>
+  <si>
+    <t>A Japanese-American classic roll. Simple Sushi dish</t>
+  </si>
+  <si>
+    <t>Thaw imitation crab. Wash and cook rice. Place imitation crab and mayo in a large bowl. Add pepper to the mixture. Wash cucumbers. Cut and grate cucumber to small thin slices with a Japanese slicer. Cut the remainder of the cucumber when it is too small to grate. Slice avocado long way around the seed. Cut seaweed into 4s.</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8338/8246846854_e6b7652a75_b.jpg</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Wasabi</t>
+  </si>
+  <si>
+    <t>Meatball Sandwich &amp; Salad</t>
+  </si>
+  <si>
+    <t>Fast and easy meatball sandwich</t>
+  </si>
+  <si>
+    <t>Preheat oven to 375. Place meatballs in aluminum tray (1 bag per tray) and bake for 45 minutes. Pour pasta sauce into a pot and heat. Add meatballs into pot.</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8338/8245824377_7a70a3d2ca.jpg</t>
+  </si>
+  <si>
+    <t>Pasta Sauce</t>
+  </si>
+  <si>
+    <t>Shredded Mozarella Cheese</t>
+  </si>
+  <si>
+    <t>Roma Tomatoes</t>
+  </si>
+  <si>
+    <t>Chicken Teriyaki &amp; Salad</t>
+  </si>
+  <si>
+    <t>Chicken Teriyaki with a traditional house salad</t>
+  </si>
+  <si>
+    <t>Preheat oven to 400 degrees. Lay out chicken in aluminum tray and bake in the oven. Cut cucumbers into half-moons and tomatoes into wedges. Mix the vegetables together along with the salad.</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8063/8245320825_24dcfaf2e9_z.jpg</t>
+  </si>
+  <si>
+    <t>Tyson Teriyaki Chicken Thighs</t>
+  </si>
+  <si>
+    <t>Balsamic Vinaigrette</t>
+  </si>
+  <si>
+    <t>Soy Sauce Chicken &amp; Salad</t>
+  </si>
+  <si>
+    <t>Korean-style chicken over rice with a traditional house salad</t>
+  </si>
+  <si>
+    <t>Mix soy sauce, sugar, and water in a 1:1:1 ratio and stir together. Place mixture in a pot and bring to a boil. Add chicken to the pot when boiling. You can also add potatoes and baby carrots if you want. You should use 10 pounds of potatoes and 5 pounds of carrots per 40 people. Cut cucumbers into half-moons and tomatoes into wedges. Mix the vegetables together along with the salad mix. Make sure the chicken is thoroughly cooked.</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8202/8248191796_25abe0d73d_b.jpg</t>
+  </si>
+  <si>
+    <t>Chicken Thighs</t>
   </si>
 </sst>
 </file>
@@ -721,6 +901,20 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -742,20 +936,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -807,7 +987,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:C1048576"/>
   <tableColumns count="3">
     <tableColumn id="1" name="cooked_meal"/>
@@ -1105,19 +1285,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1141,7 +1321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1161,23 +1341,163 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="D3" s="1">
+        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="1">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="1">
+        <v>75</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1192,28 +1512,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,7 +1541,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4">
         <v>16</v>
@@ -1232,7 +1552,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" s="7">
         <v>150</v>
@@ -1243,7 +1563,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4">
         <v>12</v>
@@ -1254,7 +1574,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7">
         <v>8</v>
@@ -1265,7 +1585,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4">
         <v>16</v>
@@ -1276,7 +1596,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7">
         <v>8</v>
@@ -1287,32 +1607,703 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4">
         <v>25</v>
       </c>
-      <c r="C9" s="7">
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40">
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
+      <c r="C66">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>